<commit_message>
Add Laubrock + Kliegl
</commit_message>
<xml_diff>
--- a/literature/lit-review_readAloud-valence-dataset.xlsx
+++ b/literature/lit-review_readAloud-valence-dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessraissouni/github/brainBox/brainy-ideas/readAloud-valence-jess/literature/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessraissouni/github/readAloud-valence-dataset/literature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C041E9-E693-B640-8635-CDA1722823FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A9A8AF-323F-1748-9D64-0D05E24E72F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="500" windowWidth="28760" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="219">
   <si>
     <t>Citation</t>
   </si>
@@ -1336,6 +1336,30 @@
   </si>
   <si>
     <t>Interesting to note that authors here did not see a significant different in behavioral results between negative and neutral congruent trials.</t>
+  </si>
+  <si>
+    <t>Laubrock, J., &amp; Kliegl, R. (2015). The eye-voice span during reading aloud. Frontiers in Psychology, 0. https://doi.org/10.3389/fpsyg.2015.01432</t>
+  </si>
+  <si>
+    <t>Temporal and spatial EVS had lower interindividual variation than intraindividual variation; by offset ~254ms/9.7 letters, by onset ~561ms/16.2 letters.</t>
+  </si>
+  <si>
+    <t>Difficult words (low frequency or low predictability) require more processing and therefore lead to refixations, which attenuate the EVS.</t>
+  </si>
+  <si>
+    <t>Authors perform oral and silent reading tasks on the same set of German sentences (different participant groups) to perform exploratory analyses on the eye-voice span (EVS).  They find evidence that the oculomotor system is regulated by the cognitive system, with a relatively stable amount of information stored in (pre-articulatory) working memory. Given that this buffer is constantly updating during oral reading, online control is required, determining the when and where of "corrective" eye movements within the text.</t>
+  </si>
+  <si>
+    <t>When the EVS gets too large, two processes seek to correct the gap: refixations/longer fixations and, when fixation time is insufficient to control an expanding EVS, regressive eye movements.</t>
+  </si>
+  <si>
+    <t>By the time a participant begins processing the switch word, they will be articulating ~16 letters prior in the text.  This aligns well with the study design establishing the switch group as the switch word and two words prior/following and the preswitch group as the five words preceding the switch group, to ensure that behavioral effects related to the switch are seen either when the switch word is first fixated (at which time the voice will be articulating words in the preswitch group) or when articulation of the switch word is prepared/performed (switch group).  Given the assumptions about the working memory buffer here, it seems unlikely that behavioral effects will be seen very long after articulation of the switch word (that is, in the postswitch group).</t>
+  </si>
+  <si>
+    <t>"...the overall pattern of results suggests that the EVS is quite flexible, and is adjusted according to cognitive, oculomotor, and articulatory demands. Given that the voice proceeds fairly linearly through the text, most of the adjustment is actually performed by the oculomotor system. The eyes, and also the mind, could in principle proceed faster than the voice, since silent reading is faster than oral reading. However, the eyes need to wait for the voice because the size of the working memory buffer is limited. The major target value in the system controlling the eyes during oral reading is a constant EVS at fixation offset of about 10 letters, translating into an average temporal EVS of about 560 ms..."</t>
+  </si>
+  <si>
+    <t>What can the eye-voice span tell us about eye movement behavior during reading?  What factors affect the EVS?</t>
   </si>
 </sst>
 </file>
@@ -1774,11 +1798,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2400,6 +2424,32 @@
       </c>
       <c r="H24" s="3" t="s">
         <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Crosscheck consistency of variable names
</commit_message>
<xml_diff>
--- a/literature/lit-review_readAloud-valence-dataset.xlsx
+++ b/literature/lit-review_readAloud-valence-dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessraissouni/github/readAloud-valence-dataset/literature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678CFE7F-7CCA-8140-800A-1DE62EF557FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF994A0-0865-524E-8CB4-0DCD6B0D05BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1008,230 +1008,230 @@
 "Typically, when two factors exert an interactive effect on word recognition, those factors are assumed to arise at the same stage of processing: If the two factors operated at different processing stages, it is unclear how they could interact. So given that frequency effects arise at the lexico-semantic stage of processing, and that frequency interacts with emotional factors, those emotional effects presumably also arise at the lexico- semantic stage."</t>
   </si>
   <si>
-    <t>Authors analyze lexical decision and naming latencies in the ELP using three large corpora (BUTLEX-US, HAL, TASA12) for frequency distributions and valence ratings from a dataset more closely aligned with natural language (Warriner et al., 2013) than ANEW (or Kousta et al.'s 2009 extension thereof). They seek to shed light on the conflicting findings of prior studies, which were limited in the size of their word set, controlled for differing sets of factors, and did not always test interaction effects.  Their analyses reveal six key findings:
+    <t>Prior studies conflict on the shape of the relationship between valence and word recognition: monotonic step-function, monotonic linear, or inverted-U.  This mega-study finds, when valence x frequency interactions are taken into account, valence has a negative relationship to behavioral latency and the magnitude of the effect is attenuated as frequency increases. (To wit: faster RT for lower frequency positive words than negative, but less distinction for higher frequency words.)</t>
+  </si>
+  <si>
+    <t>Prior studies conflict on whether valence and arousal independently influence word recognition, whether they interact in their effect, or whether only valence (not arousal) has any effect. This mega-study finds, when arousal x frequency interactions are taken into account, arousal has a positive relationship to behavioral latency and the magnitude of the effect is attenuated as frequency increases. The study also finds that the affective properties of valence and arousal have independent effects.</t>
+  </si>
+  <si>
+    <t>Strong theoretical background on automatic vigilance, including lexico-semantic and decision-response explanations thereof.</t>
+  </si>
+  <si>
+    <t>1. How will the presentation (all words on screen at once) affect participants' ability to plan encoding?
+2. How can we control for speaking rate?</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;Note that Kuperman et al. (2014) contradicts this after taking valence x frequency effects into account.</t>
+  </si>
+  <si>
+    <t>If we want to report or control for arousal norms, can we get this improved database to add to ANEW?
+&gt;&gt;&gt;These findings are nullified by the more detailed analyses of Kuperman et al. (2014).  Will use Warriner et al. (2013) instead.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Assumption #1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> reading a narrative is an assimilative process and therefore good mood will facilitate performance on the reading aloud task.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Assumption #2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>positive mood-congruency leads to lower N400 amplitudes and more efficient priming; therefore, we should see improved performance in the positive/positive context.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. It will be important to include cumulative surprisal/predictability in our models, both for the passage parts, as well as for the switch words.
+2. When we calculate surprisal, do we find that the valence shifts are more surprising (that is, less likely in the ngram context)?</t>
+  </si>
+  <si>
+    <t>What happens if one reruns the Larsen et al. (2006) analyses using a consistent measure of valence?</t>
+  </si>
+  <si>
+    <t>Estes, Z., &amp; Adelman, J. S. (2008). Automatic vigilance for negative words in lexical decision and naming: Comment on Larsen, Mercer, and Balota (2006). Emotion, 8(4), 441–444. https://doi.org/10.1037/1528-3542.8.4.441</t>
+  </si>
+  <si>
+    <t>This paper is a revised analysis of that undertaken by Larsen et al. (2006), which found that, once sublexical characteristics such as frequency are accounted for in a meta-analysis of 32 emotional Stroop tasks, negative words do not slow lexical decision or naming relative to neutral controls.  Authors here continued to use the English Lexicon Project (ELP) for lexical decision and word naming data, but imposed consistency on the valence rating measure by using the ANEW database.  (For frequency data, they relied upon the TASA12 corpus.)  Their revised analysis reveals that, particularly when valence is considered categorically (rather than linearly), responses are, indeed, slowed for negative words.</t>
+  </si>
+  <si>
+    <t>The Larsen et al. (2006) paper uses lexical decision and word naming data from the ELP, which had a standardized methodology.  However, Larsen et al. (2006) adopted the valence measure of each individual study in which it was used, which therefore may reduce statistical sensitivity.  Authors here use the ELP, but with ANEW for valence ratings.</t>
+  </si>
+  <si>
+    <t>Revised analysis finds that valence does not contribute to accuracy, but that negative words slowed lexical decision and naming.  Specifically, they find that a categorical (rather than continuous) model provides a better fit (namely, the fact of a word's valence as either positive or negative is more relevant than how far from the midpoint its valence lies).</t>
+  </si>
+  <si>
+    <t>Larsen et al. (2006) found no evidence that negative words were slowed compared to neutral.  Authors here posit that the reason for their divergent findings is that Larsen et al.'s dataset included &gt;33% neutral words and, given that effect of valence is categorical rather than linear, the neutral items were actually either slightly positive or slightly negative, obscuring the results.</t>
+  </si>
+  <si>
+    <t>"The categorical nature of this effect suggests that affective evaluation is fast but crude (Pratto &amp; John, 1991). Evidently, one immediately categorizes a stimulus as negative or positive (Fazio, 2001; Lazarus, 1982; Zajonc, 1980), and this categorical evalua- tion affects one’s response. If the stimulus is positive, then re- sponding generally proceeds rapidly. But if the stimulus is nega- tive, then responses to other aspects of the stimulus (such as its color, its pronunciation, or its lexical status) are delayed."</t>
+  </si>
+  <si>
+    <t>Four different potential relationships between word recognition and automatic vigilance can be envisaged: (1) binary, categorical judgment of stimuli as aversive or appetitive; (2) gradient judgments of valence across the spectrum; (3) motivational relevance in place of automatic vigilance, such that valenced words (positive or negative) receive preferential processing; or (4) interaction between valence and arousal (e.g. high arousal + negative should receive fastest processing).  Authors findings here support #2, and these effects held not only across times but also across individual trials.</t>
+  </si>
+  <si>
+    <t>Contradiction of Larsen et al. (2006) finding that negative words are not delayed in comparison to neutral.
+Finds that effect of valence on behavioral latency is categorical (not linear), but this is contradicted later by Kuperman et al. (2014).
+Authors argue that ANEW database is reliable for valence ratings, but these findings are contradicted later by Kousta et al. (2009).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(Estes and Adelman, 2008)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">    -length
+    -frequency
+    -contextual diversity
+    -orthographic neighborhood
+    -initial phoneme
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(English, mega-sample from ELP, non-replication of Larsen et al. by using consistent measure of valence (ANEW), also find that valence effect is categorical rather than linear)</t>
+    </r>
+  </si>
+  <si>
+    <t>Balota, D. A., Yap, M. J., Hutchison, K. A., Cortese, M. J., Kessler, B., Loftis, B., Neely, J. H., Nelson, D. L., Simpson, G. B., &amp; Treiman, R. (2007). The English Lexicon Project. Behavior Research Methods, 39(3), 445–459. https://doi.org/10.3758/BF03193014</t>
+  </si>
+  <si>
+    <t>Introduction to the English Lexicon Project (ELP).</t>
+  </si>
+  <si>
+    <t>This paper describes the purpose and methodology of the English Lexicon Project, a multi-university endeavor culminating in standardized descriptive and behavioral data for 40,481 English words (and 40,481 nonwords) based on data fro 816 participants for lexical decision and 444 participants for speeded naming.  The paper also details how to use the ELP's web interface.</t>
+  </si>
+  <si>
+    <t>Not all possible derivations of a given stem are included, although efforts were made to include the most common derivations.</t>
+  </si>
+  <si>
+    <t>For speeded naming, participants actually coded their own data (correct pronunciation, uncertain of pronunciation, incorrect pronunciation, microphone error).</t>
+  </si>
+  <si>
+    <t>"In summary, the ELP is potentially useful for equating items across a wide variety of research enterprises that use words as the primary stimulus. Obviously, for a number of reasons, the lexical characteristics included in the ELP are not, and were not meant to be, exhaustive."</t>
+  </si>
+  <si>
+    <t>Warriner, A. B., Kuperman, V., &amp; Brysbaert, M. (2013). Norms of valence, arousal, and dominance for 13,915 English lemmas. Behavior Research Methods, 45(4), 1191–1207. https://doi.org/10.3758/s13428-012-0314-x</t>
+  </si>
+  <si>
+    <t>It might be useful to analyze switch words based on valence strength (delta with neutral) as opposed to just binary neg2pos and pos2neg.</t>
+  </si>
+  <si>
+    <t>Affective ratings of ~14k lemmas to replace/extend ANEW, plus demographic and relational analyses.</t>
+  </si>
+  <si>
+    <t>Authors use mTurk to create a database of valence, arousal, and dominance ratings for English word lemmas in order to address the mismatch between the limited words available in the ANEW database and the megastudy analyses currently prevalent in psycholinguistics.  They also gather demographic information from the raters and provide information on primary correlations found.</t>
+  </si>
+  <si>
+    <t>On scales from low-to-high (unhappy/calm/controlled &gt; happy/excited/in control), distributions of valence and dominance are negatively skewed: more words make people feel happy/in control (versus unhappy/controlled) whereas arousal is positively skewed: fewer words make people feel excited.  Overall, ratings of valence were relatively consistent across participants, but arousal and dominance had higher standard deviations, indicating more variability across participant responses.</t>
+  </si>
+  <si>
+    <t>Words high on the valence scale (that make people happy) have greater imageability, concreteness, familiarity, context availability, and body-object interaction; they are also higher in frequency and learned at earlier age.  Virtually all of these same words also make people feel in control.</t>
+  </si>
+  <si>
+    <t>Across all three dimensions, younger (v. older), lower (v. higher) education, and male (v. female) gave slightly higher ratings.  Female raters provided more extreme valence and dominance ratings for words on opposing ends of the frequency spectrum, leading a broader range of ratings for valence and dominance for female raters; the relationship between frequency and arousal for female raters was weak.</t>
+  </si>
+  <si>
+    <t>"The number of words covered by the ANEW norms appeared sufficient for use in small-scale factorial experiments. In these experiments, a limited number of stimuli would be selected that varied on one dimension (e.g., valence) and were matched on other variables (e.g., arousal, word frequency, and word length). However, the number of words in this set is prohibitively small for the large-scale megastudies that are currently emerging in psycholinguistics."
+"To sum up, in terms of the variability of ratings, valence and dominance pattern together and are best considered in terms of their magnitude (how strong is the feeling) rather than their polarity (sad vs. happy, or controlled by vs. in control); polarity, however, determines variability in the arousal ratings."
+"The fact that extreme values of valence and dominance are more arousing point again at the utility of considering valence/dominance strength (i.e., how different a word is from neutral) rather than polarity as the explanatory variable."</t>
+  </si>
+  <si>
+    <t>Kanske, P., &amp; Kotz, S. A. (2011). Emotion Speeds up Conflict Resolution: A New Role for the Ventral Anterior Cingulate Cortex? Cerebral Cortex, 21(4), 911–919. https://doi.org/10.1093/cercor/bhq157</t>
+  </si>
+  <si>
+    <t>What role does the vACC play in conflict resolution when stimuli are negative (v neutral)?</t>
+  </si>
+  <si>
+    <t>Authors review behavioral, ERP, and fMRI data in a modified Simon task in which participants were tasked with a voice gender decision for words (either negatively valenced or neutral, with matching prosody) presented in either left or right ear; response key for voice gender was congruent with presentation side for congruent trials and incongruent with presentation side for conflict trials.  They find differential engagement of the ACC (anterior cingulate cortex) when processing conflict in an affective context: the dACC (dorsal ACC) processes conflict regardless of emotion whereas the vACC (ventral ACC) is additionally recruited when stimuli are emotional.  Recruitment of the vACC is accompanied by faster behavioral conflict resolution and amplified ERP conflict negativity.</t>
+  </si>
+  <si>
+    <t>Behavioral results (both ERP and fMRI experiments): RTs for negative and neutral stimuli were not significantly different for main effects nor for congruent trials; however, RTs were significantly faster in negative incongruent trials.</t>
+  </si>
+  <si>
+    <t>ERP data: conflict negativity ~420 ms with larger amplitude for incongruent (v. congruent) trials at frontal and central sites; negativity only significant over anterior sites; interaction of emotion and conflict only significant at anterior (not posterior) electrode sites.</t>
+  </si>
+  <si>
+    <t>Enhanced activation in left and right dACC for incongruent (v. congruent) trials and activation in the right vACC for conflict in emotional trials; bilateral activation of the amgydala for negative (v. neutral) words with a main effect of emotion but no effect for conflict or conflict/emotion interaction.</t>
+  </si>
+  <si>
+    <t>"An emotional target stimulus, such as the words in the present study, will signal relevance and require a rapid response. This information alone did not have behavioral consequences; RTs in the congruent emotional and neutral conditions did not differ. However, in the incongruent condition, in which incompatible response activations competed, emotion biased selection and commitment of resources leading to reduced RTs in incongruent emotional trials."</t>
+  </si>
+  <si>
+    <t>Interesting to note that authors here did not see a significant different in behavioral results between negative and neutral congruent trials.</t>
+  </si>
+  <si>
+    <t>Laubrock, J., &amp; Kliegl, R. (2015). The eye-voice span during reading aloud. Frontiers in Psychology, 0. https://doi.org/10.3389/fpsyg.2015.01432</t>
+  </si>
+  <si>
+    <t>Temporal and spatial EVS had lower interindividual variation than intraindividual variation; by offset ~254ms/9.7 letters, by onset ~561ms/16.2 letters.</t>
+  </si>
+  <si>
+    <t>Difficult words (low frequency or low predictability) require more processing and therefore lead to refixations, which attenuate the EVS.</t>
+  </si>
+  <si>
+    <t>Authors perform oral and silent reading tasks on the same set of German sentences (different participant groups) to perform exploratory analyses on the eye-voice span (EVS).  They find evidence that the oculomotor system is regulated by the cognitive system, with a relatively stable amount of information stored in (pre-articulatory) working memory. Given that this buffer is constantly updating during oral reading, online control is required, determining the when and where of "corrective" eye movements within the text.</t>
+  </si>
+  <si>
+    <t>When the EVS gets too large, two processes seek to correct the gap: refixations/longer fixations and, when fixation time is insufficient to control an expanding EVS, regressive eye movements.</t>
+  </si>
+  <si>
+    <t>By the time a participant begins processing the switch word, they will be articulating ~16 letters prior in the text.  This aligns well with the study design establishing the switch group as the switch word and two words prior/following and the preswitch group as the five words preceding the switch group, to ensure that behavioral effects related to the switch are seen either when the switch word is first fixated (at which time the voice will be articulating words in the preswitch group) or when articulation of the switch word is prepared/performed (switch group).  Given the assumptions about the working memory buffer here, it seems unlikely that behavioral effects will be seen very long after articulation of the switch word (that is, in the postswitch group).</t>
+  </si>
+  <si>
+    <t>"...the overall pattern of results suggests that the EVS is quite flexible, and is adjusted according to cognitive, oculomotor, and articulatory demands. Given that the voice proceeds fairly linearly through the text, most of the adjustment is actually performed by the oculomotor system. The eyes, and also the mind, could in principle proceed faster than the voice, since silent reading is faster than oral reading. However, the eyes need to wait for the voice because the size of the working memory buffer is limited. The major target value in the system controlling the eyes during oral reading is a constant EVS at fixation offset of about 10 letters, translating into an average temporal EVS of about 560 ms..."</t>
+  </si>
+  <si>
+    <t>What can the eye-voice span tell us about eye movement behavior during reading?  What factors affect the EVS?</t>
+  </si>
+  <si>
+    <t>Authors analyze lexical decision and naming latencies in the ELP using three large corpora (SUBTLEX-US, HAL, TASA12) for frequency distributions and valence ratings from a dataset more closely aligned with natural language (Warriner et al., 2013) than ANEW (or Kousta et al.'s 2009 extension thereof). They seek to shed light on the conflicting findings of prior studies, which were limited in the size of their word set, controlled for differing sets of factors, and did not always test interaction effects.  Their analyses reveal six key findings:
 1) valence has a monotonic effect on word response times (negative&lt;neutral&lt;positive)
 2) arousal has a monotonic effect on word response time (arousing&lt;calming)
 3) the effect of valence is stronger than that of arousal
 4) the effects of valence and arousal are independent, not interactive
 5) both valence and arousal interact with word frequency (larger effects on lower-frequency words)
 6) both valence and arousal have strong effects on lexical decision than on naming</t>
-  </si>
-  <si>
-    <t>Prior studies conflict on the shape of the relationship between valence and word recognition: monotonic step-function, monotonic linear, or inverted-U.  This mega-study finds, when valence x frequency interactions are taken into account, valence has a negative relationship to behavioral latency and the magnitude of the effect is attenuated as frequency increases. (To wit: faster RT for lower frequency positive words than negative, but less distinction for higher frequency words.)</t>
-  </si>
-  <si>
-    <t>Prior studies conflict on whether valence and arousal independently influence word recognition, whether they interact in their effect, or whether only valence (not arousal) has any effect. This mega-study finds, when arousal x frequency interactions are taken into account, arousal has a positive relationship to behavioral latency and the magnitude of the effect is attenuated as frequency increases. The study also finds that the affective properties of valence and arousal have independent effects.</t>
-  </si>
-  <si>
-    <t>Strong theoretical background on automatic vigilance, including lexico-semantic and decision-response explanations thereof.</t>
-  </si>
-  <si>
-    <t>1. How will the presentation (all words on screen at once) affect participants' ability to plan encoding?
-2. How can we control for speaking rate?</t>
-  </si>
-  <si>
-    <t>&gt;&gt;&gt;Note that Kuperman et al. (2014) contradicts this after taking valence x frequency effects into account.</t>
-  </si>
-  <si>
-    <t>If we want to report or control for arousal norms, can we get this improved database to add to ANEW?
-&gt;&gt;&gt;These findings are nullified by the more detailed analyses of Kuperman et al. (2014).  Will use Warriner et al. (2013) instead.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Assumption #1:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> reading a narrative is an assimilative process and therefore good mood will facilitate performance on the reading aloud task.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Assumption #2: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>positive mood-congruency leads to lower N400 amplitudes and more efficient priming; therefore, we should see improved performance in the positive/positive context.</t>
-    </r>
-  </si>
-  <si>
-    <t>1. It will be important to include cumulative surprisal/predictability in our models, both for the passage parts, as well as for the switch words.
-2. When we calculate surprisal, do we find that the valence shifts are more surprising (that is, less likely in the ngram context)?</t>
-  </si>
-  <si>
-    <t>What happens if one reruns the Larsen et al. (2006) analyses using a consistent measure of valence?</t>
-  </si>
-  <si>
-    <t>Estes, Z., &amp; Adelman, J. S. (2008). Automatic vigilance for negative words in lexical decision and naming: Comment on Larsen, Mercer, and Balota (2006). Emotion, 8(4), 441–444. https://doi.org/10.1037/1528-3542.8.4.441</t>
-  </si>
-  <si>
-    <t>This paper is a revised analysis of that undertaken by Larsen et al. (2006), which found that, once sublexical characteristics such as frequency are accounted for in a meta-analysis of 32 emotional Stroop tasks, negative words do not slow lexical decision or naming relative to neutral controls.  Authors here continued to use the English Lexicon Project (ELP) for lexical decision and word naming data, but imposed consistency on the valence rating measure by using the ANEW database.  (For frequency data, they relied upon the TASA12 corpus.)  Their revised analysis reveals that, particularly when valence is considered categorically (rather than linearly), responses are, indeed, slowed for negative words.</t>
-  </si>
-  <si>
-    <t>The Larsen et al. (2006) paper uses lexical decision and word naming data from the ELP, which had a standardized methodology.  However, Larsen et al. (2006) adopted the valence measure of each individual study in which it was used, which therefore may reduce statistical sensitivity.  Authors here use the ELP, but with ANEW for valence ratings.</t>
-  </si>
-  <si>
-    <t>Revised analysis finds that valence does not contribute to accuracy, but that negative words slowed lexical decision and naming.  Specifically, they find that a categorical (rather than continuous) model provides a better fit (namely, the fact of a word's valence as either positive or negative is more relevant than how far from the midpoint its valence lies).</t>
-  </si>
-  <si>
-    <t>Larsen et al. (2006) found no evidence that negative words were slowed compared to neutral.  Authors here posit that the reason for their divergent findings is that Larsen et al.'s dataset included &gt;33% neutral words and, given that effect of valence is categorical rather than linear, the neutral items were actually either slightly positive or slightly negative, obscuring the results.</t>
-  </si>
-  <si>
-    <t>"The categorical nature of this effect suggests that affective evaluation is fast but crude (Pratto &amp; John, 1991). Evidently, one immediately categorizes a stimulus as negative or positive (Fazio, 2001; Lazarus, 1982; Zajonc, 1980), and this categorical evalua- tion affects one’s response. If the stimulus is positive, then re- sponding generally proceeds rapidly. But if the stimulus is nega- tive, then responses to other aspects of the stimulus (such as its color, its pronunciation, or its lexical status) are delayed."</t>
-  </si>
-  <si>
-    <t>Four different potential relationships between word recognition and automatic vigilance can be envisaged: (1) binary, categorical judgment of stimuli as aversive or appetitive; (2) gradient judgments of valence across the spectrum; (3) motivational relevance in place of automatic vigilance, such that valenced words (positive or negative) receive preferential processing; or (4) interaction between valence and arousal (e.g. high arousal + negative should receive fastest processing).  Authors findings here support #2, and these effects held not only across times but also across individual trials.</t>
-  </si>
-  <si>
-    <t>Contradiction of Larsen et al. (2006) finding that negative words are not delayed in comparison to neutral.
-Finds that effect of valence on behavioral latency is categorical (not linear), but this is contradicted later by Kuperman et al. (2014).
-Authors argue that ANEW database is reliable for valence ratings, but these findings are contradicted later by Kousta et al. (2009).</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(Estes and Adelman, 2008)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">    -length
-    -frequency
-    -contextual diversity
-    -orthographic neighborhood
-    -initial phoneme
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>(English, mega-sample from ELP, non-replication of Larsen et al. by using consistent measure of valence (ANEW), also find that valence effect is categorical rather than linear)</t>
-    </r>
-  </si>
-  <si>
-    <t>Balota, D. A., Yap, M. J., Hutchison, K. A., Cortese, M. J., Kessler, B., Loftis, B., Neely, J. H., Nelson, D. L., Simpson, G. B., &amp; Treiman, R. (2007). The English Lexicon Project. Behavior Research Methods, 39(3), 445–459. https://doi.org/10.3758/BF03193014</t>
-  </si>
-  <si>
-    <t>Introduction to the English Lexicon Project (ELP).</t>
-  </si>
-  <si>
-    <t>This paper describes the purpose and methodology of the English Lexicon Project, a multi-university endeavor culminating in standardized descriptive and behavioral data for 40,481 English words (and 40,481 nonwords) based on data fro 816 participants for lexical decision and 444 participants for speeded naming.  The paper also details how to use the ELP's web interface.</t>
-  </si>
-  <si>
-    <t>Not all possible derivations of a given stem are included, although efforts were made to include the most common derivations.</t>
-  </si>
-  <si>
-    <t>For speeded naming, participants actually coded their own data (correct pronunciation, uncertain of pronunciation, incorrect pronunciation, microphone error).</t>
-  </si>
-  <si>
-    <t>"In summary, the ELP is potentially useful for equating items across a wide variety of research enterprises that use words as the primary stimulus. Obviously, for a number of reasons, the lexical characteristics included in the ELP are not, and were not meant to be, exhaustive."</t>
-  </si>
-  <si>
-    <t>Warriner, A. B., Kuperman, V., &amp; Brysbaert, M. (2013). Norms of valence, arousal, and dominance for 13,915 English lemmas. Behavior Research Methods, 45(4), 1191–1207. https://doi.org/10.3758/s13428-012-0314-x</t>
-  </si>
-  <si>
-    <t>It might be useful to analyze switch words based on valence strength (delta with neutral) as opposed to just binary neg2pos and pos2neg.</t>
-  </si>
-  <si>
-    <t>Affective ratings of ~14k lemmas to replace/extend ANEW, plus demographic and relational analyses.</t>
-  </si>
-  <si>
-    <t>Authors use mTurk to create a database of valence, arousal, and dominance ratings for English word lemmas in order to address the mismatch between the limited words available in the ANEW database and the megastudy analyses currently prevalent in psycholinguistics.  They also gather demographic information from the raters and provide information on primary correlations found.</t>
-  </si>
-  <si>
-    <t>On scales from low-to-high (unhappy/calm/controlled &gt; happy/excited/in control), distributions of valence and dominance are negatively skewed: more words make people feel happy/in control (versus unhappy/controlled) whereas arousal is positively skewed: fewer words make people feel excited.  Overall, ratings of valence were relatively consistent across participants, but arousal and dominance had higher standard deviations, indicating more variability across participant responses.</t>
-  </si>
-  <si>
-    <t>Words high on the valence scale (that make people happy) have greater imageability, concreteness, familiarity, context availability, and body-object interaction; they are also higher in frequency and learned at earlier age.  Virtually all of these same words also make people feel in control.</t>
-  </si>
-  <si>
-    <t>Across all three dimensions, younger (v. older), lower (v. higher) education, and male (v. female) gave slightly higher ratings.  Female raters provided more extreme valence and dominance ratings for words on opposing ends of the frequency spectrum, leading a broader range of ratings for valence and dominance for female raters; the relationship between frequency and arousal for female raters was weak.</t>
-  </si>
-  <si>
-    <t>"The number of words covered by the ANEW norms appeared sufficient for use in small-scale factorial experiments. In these experiments, a limited number of stimuli would be selected that varied on one dimension (e.g., valence) and were matched on other variables (e.g., arousal, word frequency, and word length). However, the number of words in this set is prohibitively small for the large-scale megastudies that are currently emerging in psycholinguistics."
-"To sum up, in terms of the variability of ratings, valence and dominance pattern together and are best considered in terms of their magnitude (how strong is the feeling) rather than their polarity (sad vs. happy, or controlled by vs. in control); polarity, however, determines variability in the arousal ratings."
-"The fact that extreme values of valence and dominance are more arousing point again at the utility of considering valence/dominance strength (i.e., how different a word is from neutral) rather than polarity as the explanatory variable."</t>
-  </si>
-  <si>
-    <t>Kanske, P., &amp; Kotz, S. A. (2011). Emotion Speeds up Conflict Resolution: A New Role for the Ventral Anterior Cingulate Cortex? Cerebral Cortex, 21(4), 911–919. https://doi.org/10.1093/cercor/bhq157</t>
-  </si>
-  <si>
-    <t>What role does the vACC play in conflict resolution when stimuli are negative (v neutral)?</t>
-  </si>
-  <si>
-    <t>Authors review behavioral, ERP, and fMRI data in a modified Simon task in which participants were tasked with a voice gender decision for words (either negatively valenced or neutral, with matching prosody) presented in either left or right ear; response key for voice gender was congruent with presentation side for congruent trials and incongruent with presentation side for conflict trials.  They find differential engagement of the ACC (anterior cingulate cortex) when processing conflict in an affective context: the dACC (dorsal ACC) processes conflict regardless of emotion whereas the vACC (ventral ACC) is additionally recruited when stimuli are emotional.  Recruitment of the vACC is accompanied by faster behavioral conflict resolution and amplified ERP conflict negativity.</t>
-  </si>
-  <si>
-    <t>Behavioral results (both ERP and fMRI experiments): RTs for negative and neutral stimuli were not significantly different for main effects nor for congruent trials; however, RTs were significantly faster in negative incongruent trials.</t>
-  </si>
-  <si>
-    <t>ERP data: conflict negativity ~420 ms with larger amplitude for incongruent (v. congruent) trials at frontal and central sites; negativity only significant over anterior sites; interaction of emotion and conflict only significant at anterior (not posterior) electrode sites.</t>
-  </si>
-  <si>
-    <t>Enhanced activation in left and right dACC for incongruent (v. congruent) trials and activation in the right vACC for conflict in emotional trials; bilateral activation of the amgydala for negative (v. neutral) words with a main effect of emotion but no effect for conflict or conflict/emotion interaction.</t>
-  </si>
-  <si>
-    <t>"An emotional target stimulus, such as the words in the present study, will signal relevance and require a rapid response. This information alone did not have behavioral consequences; RTs in the congruent emotional and neutral conditions did not differ. However, in the incongruent condition, in which incompatible response activations competed, emotion biased selection and commitment of resources leading to reduced RTs in incongruent emotional trials."</t>
-  </si>
-  <si>
-    <t>Interesting to note that authors here did not see a significant different in behavioral results between negative and neutral congruent trials.</t>
-  </si>
-  <si>
-    <t>Laubrock, J., &amp; Kliegl, R. (2015). The eye-voice span during reading aloud. Frontiers in Psychology, 0. https://doi.org/10.3389/fpsyg.2015.01432</t>
-  </si>
-  <si>
-    <t>Temporal and spatial EVS had lower interindividual variation than intraindividual variation; by offset ~254ms/9.7 letters, by onset ~561ms/16.2 letters.</t>
-  </si>
-  <si>
-    <t>Difficult words (low frequency or low predictability) require more processing and therefore lead to refixations, which attenuate the EVS.</t>
-  </si>
-  <si>
-    <t>Authors perform oral and silent reading tasks on the same set of German sentences (different participant groups) to perform exploratory analyses on the eye-voice span (EVS).  They find evidence that the oculomotor system is regulated by the cognitive system, with a relatively stable amount of information stored in (pre-articulatory) working memory. Given that this buffer is constantly updating during oral reading, online control is required, determining the when and where of "corrective" eye movements within the text.</t>
-  </si>
-  <si>
-    <t>When the EVS gets too large, two processes seek to correct the gap: refixations/longer fixations and, when fixation time is insufficient to control an expanding EVS, regressive eye movements.</t>
-  </si>
-  <si>
-    <t>By the time a participant begins processing the switch word, they will be articulating ~16 letters prior in the text.  This aligns well with the study design establishing the switch group as the switch word and two words prior/following and the preswitch group as the five words preceding the switch group, to ensure that behavioral effects related to the switch are seen either when the switch word is first fixated (at which time the voice will be articulating words in the preswitch group) or when articulation of the switch word is prepared/performed (switch group).  Given the assumptions about the working memory buffer here, it seems unlikely that behavioral effects will be seen very long after articulation of the switch word (that is, in the postswitch group).</t>
-  </si>
-  <si>
-    <t>"...the overall pattern of results suggests that the EVS is quite flexible, and is adjusted according to cognitive, oculomotor, and articulatory demands. Given that the voice proceeds fairly linearly through the text, most of the adjustment is actually performed by the oculomotor system. The eyes, and also the mind, could in principle proceed faster than the voice, since silent reading is faster than oral reading. However, the eyes need to wait for the voice because the size of the working memory buffer is limited. The major target value in the system controlling the eyes during oral reading is a constant EVS at fixation offset of about 10 letters, translating into an average temporal EVS of about 560 ms..."</t>
-  </si>
-  <si>
-    <t>What can the eye-voice span tell us about eye movement behavior during reading?  What factors affect the EVS?</t>
   </si>
 </sst>
 </file>
@@ -1676,8 +1676,8 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1863,7 +1863,7 @@
         <v>58</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>36</v>
@@ -1965,7 +1965,7 @@
         <v>69</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>70</v>
@@ -1991,7 +1991,7 @@
         <v>76</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>77</v>
@@ -2017,7 +2017,7 @@
         <v>85</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>84</v>
@@ -2144,7 +2144,7 @@
         <v>155</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>157</v>
@@ -2158,19 +2158,19 @@
         <v>160</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>166</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>162</v>
@@ -2178,129 +2178,129 @@
     </row>
     <row r="20" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>54</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="380" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="F22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="G23" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="288" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="E24" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="H24" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2406,7 +2406,7 @@
     <row r="7" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
       <c r="B7" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>100</v>

</xml_diff>